<commit_message>
transp files and bfpat
</commit_message>
<xml_diff>
--- a/InputData/trans/AVMC/Annual Vehicle Maint Cost.xlsx
+++ b/InputData/trans/AVMC/Annual Vehicle Maint Cost.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\RMI_all_states\OK\trans\AVMC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{87EC45ED-1970-44E3-962D-7FF61446FE5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{531A7B14-1B84-4D41-94BA-366A53756FF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="165" windowWidth="20895" windowHeight="16965" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12720" yWindow="285" windowWidth="15915" windowHeight="16410" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -1977,7 +1977,7 @@
         <v>143</v>
       </c>
       <c r="C1" s="25">
-        <v>44837</v>
+        <v>44944</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -5004,32 +5004,32 @@
         <v>5</v>
       </c>
       <c r="B5" s="5">
-        <f>'Cost Data'!$C83/10</f>
-        <v>243411.80622207024</v>
+        <f>'Cost Data'!$C83</f>
+        <v>2434118.0622207024</v>
       </c>
       <c r="C5" s="5">
-        <f>'Cost Data'!$B83/10</f>
-        <v>333211.96733545553</v>
+        <f>'Cost Data'!$B83</f>
+        <v>3332119.6733545554</v>
       </c>
       <c r="D5" s="5">
-        <f>'Cost Data'!$B83/10</f>
-        <v>333211.96733545553</v>
+        <f>'Cost Data'!$B83</f>
+        <v>3332119.6733545554</v>
       </c>
       <c r="E5" s="5">
-        <f>'Cost Data'!$B83/10</f>
-        <v>333211.96733545553</v>
+        <f>'Cost Data'!$B83</f>
+        <v>3332119.6733545554</v>
       </c>
       <c r="F5" s="5">
-        <f>'Cost Data'!$B83/10</f>
-        <v>333211.96733545553</v>
+        <f>'Cost Data'!$B83</f>
+        <v>3332119.6733545554</v>
       </c>
       <c r="G5" s="5">
-        <f>'Cost Data'!$B83/10</f>
-        <v>333211.96733545553</v>
+        <f>'Cost Data'!$B83</f>
+        <v>3332119.6733545554</v>
       </c>
       <c r="H5" s="5">
-        <f>'Cost Data'!$C83/10</f>
-        <v>243411.80622207024</v>
+        <f>'Cost Data'!$C83</f>
+        <v>2434118.0622207024</v>
       </c>
     </row>
     <row r="6" spans="1:8">

</xml_diff>